<commit_message>
se agrega el StartVPN.bat al proyecto y recordings para DataChangeMovilidad
</commit_message>
<xml_diff>
--- a/CargaInicial/Carga_Datos_General.xlsx
+++ b/CargaInicial/Carga_Datos_General.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\PruebaConsola\DataSources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\CargaInicial\CargaInicial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34EFD47-CCDD-42C1-96FB-A7C2AE115A40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14127961-10D7-41DB-9DB2-A78EC4D253F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -421,7 +421,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
se modif Carga_Datos_General.xlsx para ejecutar en QA4
</commit_message>
<xml_diff>
--- a/CargaInicial/Carga_Datos_General.xlsx
+++ b/CargaInicial/Carga_Datos_General.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\CargaInicial\CargaInicial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14127961-10D7-41DB-9DB2-A78EC4D253F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8892D6-3690-416C-97AA-6D2DC98B3236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -421,7 +421,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +444,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -455,7 +455,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -466,7 +466,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -477,7 +477,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -488,7 +488,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -499,7 +499,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -521,7 +521,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
se modif CargaInicial/Carga_Datos_General.xlsx para ejecutar en QA2
</commit_message>
<xml_diff>
--- a/CargaInicial/Carga_Datos_General.xlsx
+++ b/CargaInicial/Carga_Datos_General.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maruiz\Documents\Ranorex\RanorexStudio Projects\CargaInicial\CargaInicial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8892D6-3690-416C-97AA-6D2DC98B3236}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF93F2A9-B9C4-4706-97B1-435F9065E294}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -421,7 +421,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +444,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -455,7 +455,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -466,7 +466,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -477,7 +477,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -488,7 +488,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -499,7 +499,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -510,7 +510,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -521,7 +521,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>

</xml_diff>